<commit_message>
Deploying to gh-pages from @ NIH-NCPI/ncpi-fhir-ig@c278f5ec0a32a41ac6d3150126446bf42a2e3ef5 🚀
</commit_message>
<xml_diff>
--- a/CodeSystem-ConditionInheritanceMode.xlsx
+++ b/CodeSystem-ConditionInheritanceMode.xlsx
@@ -24,13 +24,13 @@
     <t>URL</t>
   </si>
   <si>
-    <t>https://ncpi-fhir.github.io/ncpi-fhir-ig/CodeSystem/ConditionInheritanceMode</t>
+    <t>https://nih-ncpi.github.io/ncpi-fhir-ig/CodeSystem/ConditionInheritanceMode</t>
   </si>
   <si>
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.0</t>
+    <t>0.2.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-08-23T15:00:44+00:00</t>
+    <t>2022-09-13T16:54:38+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ NIH-NCPI/ncpi-fhir-ig@1a96c69707a70b7f9f8c0f5682f02bcb3e5ceb5f 🚀
</commit_message>
<xml_diff>
--- a/CodeSystem-ConditionInheritanceMode.xlsx
+++ b/CodeSystem-ConditionInheritanceMode.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-12-09T17:30:30+00:00</t>
+    <t>2023-09-15T20:59:49+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -75,7 +75,7 @@
     <t>Jurisdiction</t>
   </si>
   <si>
-    <t>World</t>
+    <t>Global (Whole world)</t>
   </si>
   <si>
     <t>Description</t>
@@ -404,10 +404,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true" applyFont="true">
       <alignment vertical="top" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>

</xml_diff>